<commit_message>
- kmeans lab, caching spreadsheet [2:00]
</commit_message>
<xml_diff>
--- a/03-rdd/caching-worksheet.xlsx
+++ b/03-rdd/caching-worksheet.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sujee/ElephantScale/spark-labs/03-rdd/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="7200" yWindow="2080" windowWidth="32240" windowHeight="16980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t xml:space="preserve">data size </t>
   </si>
@@ -28,9 +36,6 @@
   </si>
   <si>
     <t>overhead</t>
-  </si>
-  <si>
-    <t>&lt;-- examine 'spark shell UI' --&gt;  'storage' tab</t>
   </si>
   <si>
     <t>after cache 1</t>
@@ -58,6 +63,21 @@
   </si>
   <si>
     <t>&lt;-- note from spark shell logs in console</t>
+  </si>
+  <si>
+    <t>RDD</t>
+  </si>
+  <si>
+    <t>DataSet</t>
+  </si>
+  <si>
+    <t>Datset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;-- 'Storage' tab </t>
+  </si>
+  <si>
+    <t>in Spark UI 4040</t>
   </si>
 </sst>
 </file>
@@ -112,7 +132,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -126,28 +146,42 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -158,16 +192,68 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
+      <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="18"/>
+      <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Time</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -181,19 +267,120 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$5</c:f>
+              <c:f>Sheet1!$B$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>time (secs)</c:v>
+                  <c:v>RDD</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$12:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DataSet</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$6:$B$11</c:f>
+              <c:f>Sheet1!$C$12:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -209,21 +396,55 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="-2141543800"/>
-        <c:axId val="-2141518008"/>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1984098352"/>
+        <c:axId val="1984099712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2141543800"/>
+        <c:axId val="1984098352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2141518008"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1984099712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -231,57 +452,1721 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2141518008"/>
+        <c:axId val="1984099712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2141543800"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1984098352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Memory</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Usage</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Actual Size</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>RDD</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Datset</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$C$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Cached Size</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>RDD</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Datset</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$C$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1985220704"/>
+        <c:axId val="2025104592"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1985220704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2025104592"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2025104592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1985220704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>359277</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>8522</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>314827</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>170447</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -291,6 +2176,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>782053</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>394367</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>160421</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -621,95 +2536,133 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="190" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B2" s="3">
+        <v>100</v>
+      </c>
+      <c r="C2" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <v>100</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <f>B2/B1</f>
-        <v>1</v>
+      <c r="B4" s="3">
+        <f>B3/B2</f>
+        <v>0</v>
+      </c>
+      <c r="C4" s="3">
+        <f>C3/C2</f>
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C10" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="C11" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>9</v>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>